<commit_message>
Methods getNumberOfRows, getNumberOfCells, LoadData and RunTest Completed
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Test</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>vOutData</t>
+  </si>
+  <si>
+    <t>aqui</t>
+  </si>
+  <si>
+    <t>CT 04</t>
+  </si>
+  <si>
+    <t>CT 05</t>
   </si>
 </sst>
 </file>
@@ -102,7 +114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -132,201 +144,57 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,104 +501,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="5">
+        <f>DATE(2020,4,13)</f>
+        <v>43934</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G3" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F4"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Test is interact with spreadsheet correctly!
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Test</t>
   </si>
@@ -64,19 +64,25 @@
     <t>Carlos Anthony</t>
   </si>
   <si>
+    <t>vOutData</t>
+  </si>
+  <si>
+    <t>aqui</t>
+  </si>
+  <si>
+    <t>CT 04</t>
+  </si>
+  <si>
+    <t>CT 05</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>vOutData</t>
-  </si>
-  <si>
-    <t>aqui</t>
-  </si>
-  <si>
-    <t>CT 04</t>
-  </si>
-  <si>
-    <t>CT 05</t>
+    <t>jordana</t>
+  </si>
+  <si>
+    <t>carlos</t>
   </si>
 </sst>
 </file>
@@ -504,7 +510,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,7 +543,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -569,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -581,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>2</v>
@@ -604,16 +610,16 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -625,7 +631,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1">
         <v>4</v>
@@ -633,10 +639,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -648,10 +654,10 @@
         <v>9</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
method to create a ExcelBackup and also Update cells of Excel
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Test</t>
   </si>
@@ -67,9 +67,6 @@
     <t>vOutData</t>
   </si>
   <si>
-    <t>aqui</t>
-  </si>
-  <si>
     <t>CT 04</t>
   </si>
   <si>
@@ -83,12 +80,16 @@
   </si>
   <si>
     <t>carlos</t>
+  </si>
+  <si>
+    <t>22/04/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,11 +183,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -200,7 +276,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -510,17 +598,17 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.90625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="18.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -547,7 +635,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -565,13 +653,12 @@
       <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="5">
-        <f>DATE(2020,4,13)</f>
-        <v>43934</v>
+      <c r="G2" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -587,14 +674,14 @@
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -610,16 +697,18 @@
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
+      <c r="A5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -631,33 +720,33 @@
         <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working in treatments of Exceptions
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>Test</t>
   </si>
@@ -83,6 +83,33 @@
   </si>
   <si>
     <t>22/04/2020</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>25_04_2020--19_13_26 891</t>
+  </si>
+  <si>
+    <t>25_04_2020--19_14_17 408</t>
+  </si>
+  <si>
+    <t>25_04_2020--19_14_48 020</t>
+  </si>
+  <si>
+    <t>25_04_2020--19_21_19 624</t>
+  </si>
+  <si>
+    <t>25_04_2020--19_25_34 264</t>
+  </si>
+  <si>
+    <t>25_04_2020--19_26_48 617</t>
   </si>
 </sst>
 </file>
@@ -595,23 +622,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.6328125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="9.90625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="18.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.90625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.90625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.81640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="25.36328125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -619,22 +648,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -642,110 +674,121 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>21</v>
+      <c r="H2" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>21</v>
+      <c r="H3" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>21</v>
+      <c r="H4" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="8"/>
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Resolved some problems and set a Header and Footer to be show in console of IDE
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Test</t>
   </si>
@@ -49,67 +49,70 @@
     <t>Lelles Moreira</t>
   </si>
   <si>
+    <t>Jordana</t>
+  </si>
+  <si>
+    <t>CT 02</t>
+  </si>
+  <si>
+    <t>CT 03</t>
+  </si>
+  <si>
+    <t>Carlos Anthony</t>
+  </si>
+  <si>
+    <t>vOutData</t>
+  </si>
+  <si>
+    <t>CT 04</t>
+  </si>
+  <si>
+    <t>CT 05</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>jordana</t>
+  </si>
+  <si>
+    <t>carlos</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>27_04_2020--21_35_53 055</t>
+  </si>
+  <si>
     <t>uilen</t>
   </si>
   <si>
-    <t>Jordana</t>
-  </si>
-  <si>
-    <t>CT 02</t>
-  </si>
-  <si>
-    <t>CT 03</t>
-  </si>
-  <si>
-    <t>Carlos Anthony</t>
-  </si>
-  <si>
-    <t>vOutData</t>
-  </si>
-  <si>
-    <t>CT 04</t>
-  </si>
-  <si>
-    <t>CT 05</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>jordana</t>
-  </si>
-  <si>
-    <t>carlos</t>
-  </si>
-  <si>
-    <t>22/04/2020</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>25_04_2020--19_13_26 891</t>
-  </si>
-  <si>
-    <t>25_04_2020--19_14_17 408</t>
-  </si>
-  <si>
-    <t>25_04_2020--19_14_48 020</t>
-  </si>
-  <si>
-    <t>25_04_2020--19_21_19 624</t>
-  </si>
-  <si>
-    <t>25_04_2020--19_25_34 264</t>
-  </si>
-  <si>
-    <t>25_04_2020--19_26_48 617</t>
+    <t>27_04_2020--23_30_35 334</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_31_17 217</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_31_47 245</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_32_25 457</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_34_44 824</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_35_37 790</t>
+  </si>
+  <si>
+    <t>27_04_2020--23_36_08 311</t>
   </si>
 </sst>
 </file>
@@ -625,7 +628,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -663,7 +666,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -674,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -686,110 +689,114 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="D6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transforming some classes and features to object oriented
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Test</t>
   </si>
@@ -91,28 +91,25 @@
     <t>uilen</t>
   </si>
   <si>
-    <t>27_04_2020--23_30_35 334</t>
-  </si>
-  <si>
     <t>27_04_2020--23_31_17 217</t>
   </si>
   <si>
-    <t>27_04_2020--23_31_47 245</t>
-  </si>
-  <si>
-    <t>27_04_2020--23_32_25 457</t>
-  </si>
-  <si>
-    <t>27_04_2020--23_34_44 824</t>
+    <t>28_04_2020--21_21_41 733</t>
+  </si>
+  <si>
+    <t>28_04_2020--21_22_15 376</t>
+  </si>
+  <si>
+    <t>28_04_2020--21_22_48 271</t>
+  </si>
+  <si>
+    <t>28_04_2020--21_27_33 556</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>27_04_2020--23_35_37 790</t>
-  </si>
-  <si>
-    <t>27_04_2020--23_36_08 311</t>
+    <t>28_04_2020--21_28_27 839</t>
   </si>
 </sst>
 </file>
@@ -628,7 +625,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,7 +741,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -752,7 +749,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -770,7 +767,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -781,7 +778,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -796,7 +793,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting the implementation of the doc file creation method
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Test</t>
   </si>
@@ -110,6 +110,39 @@
   </si>
   <si>
     <t>28_04_2020--21_28_27 839</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>04_05_2020--22_20_16 082</t>
+  </si>
+  <si>
+    <t>04_05_2020--22_20_53 190</t>
+  </si>
+  <si>
+    <t>04_05_2020--22_28_42 086</t>
+  </si>
+  <si>
+    <t>04_05_2020--22_29_14 158</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_08_14 510</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_08_47 023</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_11_44 038</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_12_16 054</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_18_51 161</t>
+  </si>
+  <si>
+    <t>04_05_2020--23_19_24 375</t>
   </si>
 </sst>
 </file>
@@ -674,7 +707,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -689,7 +722,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -793,7 +826,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
File Doc is being created with success
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
   <si>
     <t>Test</t>
   </si>
@@ -94,55 +94,25 @@
     <t>27_04_2020--23_31_17 217</t>
   </si>
   <si>
-    <t>28_04_2020--21_21_41 733</t>
-  </si>
-  <si>
     <t>28_04_2020--21_22_15 376</t>
   </si>
   <si>
-    <t>28_04_2020--21_22_48 271</t>
-  </si>
-  <si>
-    <t>28_04_2020--21_27_33 556</t>
+    <t>05_05_2020--23_32_58 612</t>
+  </si>
+  <si>
+    <t>05_05_2020--23_33_31 446</t>
+  </si>
+  <si>
+    <t>05_05_2020--23_36_02 897</t>
   </si>
   <si>
     <t>Passed</t>
   </si>
   <si>
-    <t>28_04_2020--21_28_27 839</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>04_05_2020--22_20_16 082</t>
-  </si>
-  <si>
-    <t>04_05_2020--22_20_53 190</t>
-  </si>
-  <si>
-    <t>04_05_2020--22_28_42 086</t>
-  </si>
-  <si>
-    <t>04_05_2020--22_29_14 158</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_08_14 510</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_08_47 023</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_11_44 038</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_12_16 054</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_18_51 161</t>
-  </si>
-  <si>
-    <t>04_05_2020--23_19_24 375</t>
+    <t>05_05_2020--23_36_56 694</t>
+  </si>
+  <si>
+    <t>05_05_2020--23_37_26 792</t>
   </si>
 </sst>
 </file>
@@ -658,7 +628,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,7 +677,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -722,7 +692,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -756,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>21</v>
@@ -774,7 +744,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -800,7 +770,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -826,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
settings the template to evidences
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
   <si>
     <t>Test</t>
   </si>
@@ -113,6 +113,147 @@
   </si>
   <si>
     <t>05_05_2020--23_37_26 792</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_09_30 095</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_10_11 458</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_10_41 828</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_20_03 186</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_20_37 919</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_21_10 153</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_24_26 676</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_24_58 782</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_25_31 062</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_37_35 492</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_38_10 025</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_39_59 582</t>
+  </si>
+  <si>
+    <t>06_05_2020--21_40_32 516</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_03_30 782</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_04_03 722</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_05_03 353</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_19_49 321</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_20_24 240</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_26_37 206</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_27_32 588</t>
+  </si>
+  <si>
+    <t>06_05_2020--22_28_25 723</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_17_44 407</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_18_40 558</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_20_12 688</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_21_06 211</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_21_38 483</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_26_36 041</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_27_58 675</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_28_33 354</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_29_04 221</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_30_01 147</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_30_34 625</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_31_04 928</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_32_04 879</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_32_37 461</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_34_55 660</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_35_30 270</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_37_12 342</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_37_46 742</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_41_36 764</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_42_30 931</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_43_01 584</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_46_20 720</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_47_00 332</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_48_22 535</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_49_16 646</t>
+  </si>
+  <si>
+    <t>06_05_2020--23_49_48 956</t>
   </si>
 </sst>
 </file>
@@ -692,7 +833,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -744,7 +885,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -796,7 +937,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications in some methods
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
   <si>
     <t>Test</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>09_05_2020--18_04_32 522</t>
+  </si>
+  <si>
+    <t>12/05/2020</t>
   </si>
 </sst>
 </file>
@@ -845,7 +848,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -897,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -949,7 +952,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create a EvidenceDoc oriented to objects
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
   <si>
     <t>Test</t>
   </si>
@@ -91,184 +91,16 @@
     <t>uilen</t>
   </si>
   <si>
-    <t>27_04_2020--23_31_17 217</t>
-  </si>
-  <si>
     <t>28_04_2020--21_22_15 376</t>
   </si>
   <si>
-    <t>05_05_2020--23_32_58 612</t>
-  </si>
-  <si>
-    <t>05_05_2020--23_33_31 446</t>
-  </si>
-  <si>
-    <t>05_05_2020--23_36_02 897</t>
+    <t>25/05/2020</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>05_05_2020--23_36_56 694</t>
-  </si>
-  <si>
-    <t>05_05_2020--23_37_26 792</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_09_30 095</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_10_11 458</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_10_41 828</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_20_03 186</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_20_37 919</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_21_10 153</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_24_26 676</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_24_58 782</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_25_31 062</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_37_35 492</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_38_10 025</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_39_59 582</t>
-  </si>
-  <si>
-    <t>06_05_2020--21_40_32 516</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_03_30 782</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_04_03 722</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_05_03 353</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_19_49 321</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_20_24 240</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_26_37 206</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_27_32 588</t>
-  </si>
-  <si>
-    <t>06_05_2020--22_28_25 723</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_17_44 407</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_18_40 558</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_20_12 688</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_21_06 211</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_21_38 483</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_26_36 041</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_27_58 675</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_28_33 354</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_29_04 221</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_30_01 147</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_30_34 625</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_31_04 928</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_32_04 879</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_32_37 461</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_34_55 660</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_35_30 270</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_37_12 342</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_37_46 742</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_41_36 764</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_42_30 931</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_43_01 584</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_46_20 720</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_47_00 332</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_48_22 535</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_49_16 646</t>
-  </si>
-  <si>
-    <t>06_05_2020--23_49_48 956</t>
-  </si>
-  <si>
-    <t>09_05_2020--17_44_03 082</t>
-  </si>
-  <si>
-    <t>09_05_2020--17_44_51 168</t>
-  </si>
-  <si>
-    <t>09_05_2020--18_03_58 404</t>
-  </si>
-  <si>
-    <t>09_05_2020--18_04_32 522</t>
-  </si>
-  <si>
-    <t>12/05/2020</t>
   </si>
 </sst>
 </file>
@@ -784,7 +616,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,10 +662,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -848,7 +680,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -856,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -874,7 +706,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -882,10 +714,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -900,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -926,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -934,10 +766,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -952,7 +784,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>83</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
method to Create Header in doc and Set value in header
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>Test</t>
   </si>
@@ -85,9 +85,6 @@
     <t>Failed</t>
   </si>
   <si>
-    <t>27_04_2020--21_35_53 055</t>
-  </si>
-  <si>
     <t>uilen</t>
   </si>
   <si>
@@ -100,7 +97,13 @@
     <t/>
   </si>
   <si>
+    <t>26/05/2020</t>
+  </si>
+  <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>30/05/2020</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -662,10 +665,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -677,10 +680,10 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -688,7 +691,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -706,7 +709,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -717,7 +720,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -732,7 +735,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -740,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -758,7 +761,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -769,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -784,7 +787,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating some methods em class EvidenceData
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>Test</t>
   </si>
@@ -88,9 +88,6 @@
     <t>uilen</t>
   </si>
   <si>
-    <t>28_04_2020--21_22_15 376</t>
-  </si>
-  <si>
     <t>25/05/2020</t>
   </si>
   <si>
@@ -100,10 +97,10 @@
     <t>26/05/2020</t>
   </si>
   <si>
+    <t>01/06/2020</t>
+  </si>
+  <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>30/05/2020</t>
   </si>
 </sst>
 </file>
@@ -619,7 +616,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -683,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -709,7 +706,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -720,7 +717,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>13</v>
@@ -735,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -743,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>21</v>
@@ -761,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -772,7 +769,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>13</v>
@@ -787,7 +784,7 @@
         <v>19</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create a class CompareFiles
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
   <si>
     <t>Test</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>03/06/2020</t>
   </si>
 </sst>
 </file>
@@ -680,7 +683,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Criando o metodo clicar generico para elementos
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Test</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>03/06/2020</t>
+  </si>
+  <si>
+    <t>16/06/2020</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adicionando capacidade ao projeto para trabalhar com relatorios allure
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74F992E-1ED4-4BCD-A89A-B0BEA1C2830E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Test</t>
   </si>
@@ -103,16 +104,13 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>03/06/2020</t>
-  </si>
-  <si>
-    <t>16/06/2020</t>
+    <t>16/04/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -333,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,7 +371,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -408,6 +406,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -443,9 +458,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,11 +650,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -671,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -686,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -694,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
@@ -712,7 +744,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Alterando arquivo 'pom' para direcionar allures-results para a pasta 'target'
</commit_message>
<xml_diff>
--- a/data/Scenarios/scenarios.xlsx
+++ b/data/Scenarios/scenarios.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="30">
   <si>
     <t>Test</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>16/04/2021</t>
+  </si>
+  <si>
+    <t>17/04/2021</t>
   </si>
 </sst>
 </file>
@@ -703,7 +706,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -718,7 +721,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -744,7 +747,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>